<commit_message>
[PHOENIX-6081] completed official register complaint with flow
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>dataName</t>
   </si>
@@ -177,7 +177,19 @@
     <t>Chandragiri Murali Krishna</t>
   </si>
   <si>
-    <t>Grievance approval required</t>
+    <t>Funds needed to resolve the issue</t>
+  </si>
+  <si>
+    <t>juniorAssistant</t>
+  </si>
+  <si>
+    <t>Junior Assistant</t>
+  </si>
+  <si>
+    <t>D.Subramanyam</t>
+  </si>
+  <si>
+    <t>Sanctioned and shall grievance be processed</t>
   </si>
 </sst>
 </file>
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +540,7 @@
     <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -800,6 +812,23 @@
       </c>
       <c r="E17" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-6082] completed Forward/Close Grievance
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
@@ -81,18 +81,12 @@
     <t>Commissioner</t>
   </si>
   <si>
-    <t>S.Ravindra Babu ~ ADM_Commissioner_1</t>
-  </si>
-  <si>
     <t>Forward to commissioner</t>
   </si>
   <si>
     <t>commissioner1</t>
   </si>
   <si>
-    <t>S.Ravindra Babu/ADM_Commissioner_1</t>
-  </si>
-  <si>
     <t>engineer</t>
   </si>
   <si>
@@ -190,6 +184,12 @@
   </si>
   <si>
     <t>Sanctioned and shall grievance be processed</t>
+  </si>
+  <si>
+    <t>Ravindra Babu ~ ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t>Ravindra Babu/ADM_Commissioner_1</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,15 +622,15 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -639,119 +639,119 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
@@ -760,75 +760,75 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>48</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-6077] refactoring Renew License
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>dataName</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>JAGADEESH MADARAPU</t>
+  </si>
+  <si>
+    <t>commissioner2</t>
+  </si>
+  <si>
+    <t>Ravindra Babu ~ ADM_Commissioner_2</t>
   </si>
 </sst>
 </file>
@@ -528,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,6 +835,23 @@
       </c>
       <c r="E18" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-5914] CHANGES in council management
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
@@ -177,9 +177,6 @@
     <t>Sanctioned and shall grievance be processed</t>
   </si>
   <si>
-    <t>Ravindra Babu/ADM_Commissioner_1</t>
-  </si>
-  <si>
     <t>LightingSuperintendent</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Ravindra Babu ~ ADM_Commissioner_2</t>
+  </si>
+  <si>
+    <t>Ravindra Babu/ADM_Commissioner_2</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +622,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -639,7 +639,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -799,16 +799,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
       <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
       </c>
       <c r="E17" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
[PHOENIX-5999] modified modules with new approval details
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/approvalDetailsTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -162,6 +162,9 @@
     <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
   </si>
   <si>
+    <t xml:space="preserve">Forward to DEE</t>
+  </si>
+  <si>
     <t xml:space="preserve">sanitaryInspector</t>
   </si>
   <si>
@@ -220,9 +223,6 @@
   </si>
   <si>
     <t xml:space="preserve">C.Radha Krishna/ENG_Dy. Executive Engineer_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to DEE</t>
   </si>
   <si>
     <t xml:space="preserve">Executive_engineer</t>
@@ -373,17 +373,17 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.1336032388664"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -606,79 +606,82 @@
       <c r="D14" s="0" t="s">
         <v>45</v>
       </c>
+      <c r="E14" s="0" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" s="2" customFormat="true" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>26</v>
@@ -695,7 +698,7 @@
     </row>
     <row r="20" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
@@ -712,7 +715,7 @@
     </row>
     <row r="21" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>26</v>
@@ -721,10 +724,10 @@
         <v>44</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="true" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>